<commit_message>
Fix issue with which .inj files were included
</commit_message>
<xml_diff>
--- a/examples/PHIPA/experiments.xlsx
+++ b/examples/PHIPA/experiments.xlsx
@@ -673,7 +673,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>1 Injection SIM.inj</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -717,12 +717,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Plates Clean.setup</t>
+          <t>Plates Quick.setup</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>1 Injection SIM.inj</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>ChoderaHDR.inj</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -815,12 +815,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Plates Clean.setup</t>
+          <t>Plates Quick.setup</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>ChoderaHDR.inj</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>1 Injection SIM.inj</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Plates Clean.setup</t>
+          <t>Plates Quick.setup</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>1 Injection SIM.inj</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>ChoderaHDR.inj</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1109,12 +1109,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Plates Clean.setup</t>
+          <t>Plates Quick.setup</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ChoderaHSA.inj</t>
+          <t>ChoderaHDR.inj</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">

</xml_diff>

<commit_message>
New experiment plan for PHIPA! * Featuring 10, 20, 30 uM protein * New 15 mg in 10 g compound stock using latest dialysate * 150 uL syringe volumes, just in case that was a problem * assumed 40 uM affinity in designing experiment
</commit_message>
<xml_diff>
--- a/examples/PHIPA/experiments.xlsx
+++ b/examples/PHIPA/experiments.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -413,7 +413,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20191210a1.itc</t>
+          <t>20191211a1.itc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20191210a2.itc</t>
+          <t>20191211a2.itc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -511,7 +511,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20191210a3.itc</t>
+          <t>20191211a3.itc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20191210a4.itc</t>
+          <t>20191211a4.itc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>4.916364108287615</v>
+        <v>4.025027875879669</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -609,7 +609,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20191210a5.itc</t>
+          <t>20191211a5.itc</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -636,7 +636,7 @@
         <v>0.01</v>
       </c>
       <c r="G6" t="n">
-        <v>4.916364108287615</v>
+        <v>4.025027875879669</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -658,7 +658,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20191210a6.itc</t>
+          <t>20191211a6.itc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4.916364108287615</v>
+        <v>4.025027875879669</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -707,7 +707,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20191210a7.itc</t>
+          <t>20191211a7.itc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -734,7 +734,7 @@
         <v>0.01</v>
       </c>
       <c r="G8" t="n">
-        <v>4.916364108287615</v>
+        <v>4.025027875879669</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20191210a8.itc</t>
+          <t>20191211a8.itc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>4.916364108287615</v>
+        <v>4.025027875879669</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -805,7 +805,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20191210a9.itc</t>
+          <t>20191211a9.itc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -832,7 +832,7 @@
         <v>0.01</v>
       </c>
       <c r="G10" t="n">
-        <v>4.916364108287615</v>
+        <v>4.025027875879669</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -854,7 +854,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20191210a10.itc</t>
+          <t>20191211a10.itc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>5.352137824470005</v>
+        <v>4.441781158693494</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -903,7 +903,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20191210a11.itc</t>
+          <t>20191211a11.itc</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -930,7 +930,7 @@
         <v>0.02</v>
       </c>
       <c r="G12" t="n">
-        <v>5.352137824470005</v>
+        <v>4.441781158693494</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20191210a12.itc</t>
+          <t>20191211a12.itc</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>5.352137824470005</v>
+        <v>4.441781158693494</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20191210a13.itc</t>
+          <t>20191211a13.itc</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1028,7 +1028,7 @@
         <v>0.02</v>
       </c>
       <c r="G14" t="n">
-        <v>5.352137824470005</v>
+        <v>4.441781158693494</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1050,7 +1050,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20191210a14.itc</t>
+          <t>20191211a14.itc</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>5.352137824470005</v>
+        <v>4.441781158693494</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1099,7 +1099,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20191210a15.itc</t>
+          <t>20191211a15.itc</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1126,7 +1126,7 @@
         <v>0.02</v>
       </c>
       <c r="G16" t="n">
-        <v>5.352137824470005</v>
+        <v>4.441781158693494</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1148,12 +1148,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20191210a16.itc</t>
+          <t>20191211a16.itc</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>water into water</t>
+          <t>titration of Compound 46 into buffer (replicate 1)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1163,19 +1163,19 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ChoderaWaterWater.inj</t>
+          <t>ChoderaHSA.inj</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Control</t>
+          <t>Onesite</t>
         </is>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>4.816933648886398</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1191,6 +1191,300 @@
       <c r="K17" t="inlineStr">
         <is>
           <t>Plate1, G4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>20191211a17.itc</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>titration of Compound 46 into receptor (replicate 1)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Plates Clean.setup</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ChoderaHSA.inj</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G18" t="n">
+        <v>4.816933648886398</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Plate1, A5</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Plate1, B5</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Plate1, A5</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>20191211a18.itc</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SIM Compound 46 into buffer (replicate 1)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1 Injection SIM.inj</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>4.816933648886398</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Plate1, C5</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Plate1, D5</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Plate1, C5</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>20191211a19.itc</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SIM Compound 46 into receptor (replicate 1)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1 Injection SIM.inj</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4.816933648886398</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Plate1, E5</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Plate1, F5</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Plate1, E5</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20191211a20.itc</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>HDR Compound 46 into buffer (replicate 1)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ChoderaHDR.inj</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4.816933648886398</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Plate1, G5</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Plate1, H5</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Plate1, G5</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>20191211a21.itc</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>HDR Compound 46 into receptor (replicate 1)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ChoderaHDR.inj</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Onesite</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4.816933648886398</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Plate1, A6</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Plate1, B6</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Plate1, A6</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>20191211a22.itc</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>water into water</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Plates Quick.setup</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>ChoderaWaterWater.inj</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Control</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Plate1, C6</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Plate1, D6</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Plate1, C6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update openpyxl command to current version
</commit_message>
<xml_diff>
--- a/examples/PHIPA/experiments.xlsx
+++ b/examples/PHIPA/experiments.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="plate" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="plate" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -413,7 +413,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CHODERA20191219a1.itc</t>
+          <t>CHODERA20200212a1.itc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CHODERA20191219a2.itc</t>
+          <t>CHODERA20200212a2.itc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -511,7 +511,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHODERA20191219a3.itc</t>
+          <t>CHODERA20200212a3.itc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CHODERA20191219a4.itc</t>
+          <t>CHODERA20200212a4.itc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -587,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>4.633136414336804</v>
+        <v>4.633136414336805</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -609,7 +609,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CHODERA20191219a5.itc</t>
+          <t>CHODERA20200212a5.itc</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -633,10 +633,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.025</v>
+        <v>0.02500000000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>4.633136414336804</v>
+        <v>4.633136414336805</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -658,7 +658,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CHODERA20191219a6.itc</t>
+          <t>CHODERA20200212a6.itc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4.633136414336804</v>
+        <v>4.633136414336805</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -707,7 +707,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CHODERA20191219a7.itc</t>
+          <t>CHODERA20200212a7.itc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -731,10 +731,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.025</v>
+        <v>0.02500000000000001</v>
       </c>
       <c r="G8" t="n">
-        <v>4.633136414336804</v>
+        <v>4.633136414336805</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CHODERA20191219a8.itc</t>
+          <t>CHODERA20200212a8.itc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>4.633136414336804</v>
+        <v>4.633136414336805</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -805,7 +805,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CHODERA20191219a9.itc</t>
+          <t>CHODERA20200212a9.itc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -829,10 +829,10 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.025</v>
+        <v>0.02500000000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>4.633136414336804</v>
+        <v>4.633136414336805</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -854,7 +854,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CHODERA20191219a10.itc</t>
+          <t>CHODERA20200212a10.itc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -901,6 +901,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Make setup files usable, install and build works now
</commit_message>
<xml_diff>
--- a/examples/PHIPA/experiments.xlsx
+++ b/examples/PHIPA/experiments.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="plate" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="plate" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -413,7 +413,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CHODERA20200212a1.itc</t>
+          <t>CHODERA20200226a1.itc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CHODERA20200212a2.itc</t>
+          <t>CHODERA20200226a2.itc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -511,7 +511,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHODERA20200212a3.itc</t>
+          <t>CHODERA20200226a3.itc</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -560,7 +560,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CHODERA20200212a4.itc</t>
+          <t>CHODERA20200226a4.itc</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -609,7 +609,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CHODERA20200212a5.itc</t>
+          <t>CHODERA20200226a5.itc</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -658,7 +658,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CHODERA20200212a6.itc</t>
+          <t>CHODERA20200226a6.itc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -707,7 +707,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CHODERA20200212a7.itc</t>
+          <t>CHODERA20200226a7.itc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -756,7 +756,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CHODERA20200212a8.itc</t>
+          <t>CHODERA20200226a8.itc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -805,7 +805,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CHODERA20200212a9.itc</t>
+          <t>CHODERA20200226a9.itc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CHODERA20200212a10.itc</t>
+          <t>CHODERA20200226a10.itc</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -901,6 +901,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>